<commit_message>
add data to excel files
</commit_message>
<xml_diff>
--- a/excel_files/problems.xlsx
+++ b/excel_files/problems.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jscy\Desktop\bootcamp_project\Schedule-System\excel_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jscy\Desktop\bootcamp\Schedule-System\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="18">
   <si>
     <t>problem_id</t>
   </si>
@@ -46,10 +46,34 @@
     <t>Junction box that is uncovered</t>
   </si>
   <si>
-    <t>Screen freezes</t>
-  </si>
-  <si>
-    <t>Flickering light</t>
+    <t>1234A</t>
+  </si>
+  <si>
+    <t>2333B</t>
+  </si>
+  <si>
+    <t>3231R</t>
+  </si>
+  <si>
+    <t>3434T</t>
+  </si>
+  <si>
+    <t>3625N</t>
+  </si>
+  <si>
+    <t>1236G</t>
+  </si>
+  <si>
+    <t>1425F</t>
+  </si>
+  <si>
+    <t>1596D</t>
+  </si>
+  <si>
+    <t>6669R</t>
+  </si>
+  <si>
+    <t>Not working</t>
   </si>
 </sst>
 </file>
@@ -85,8 +109,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,10 +573,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,68 +607,155 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>12346</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
+        <v>12345</v>
+      </c>
+      <c r="B2" s="1">
+        <v>12345</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2">
+        <v>43795</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>22222</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
+        <v>12346</v>
+      </c>
+      <c r="B3" s="1">
+        <v>96325</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2">
+        <v>43793</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>33333</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
+        <v>12348</v>
+      </c>
+      <c r="B4" s="1">
+        <v>12347</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2">
+        <v>43794</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>44444</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
+        <v>12347</v>
+      </c>
+      <c r="B5" s="1">
+        <v>32145</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2">
+        <v>43789</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>55555</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
+        <v>12365</v>
+      </c>
+      <c r="B6" s="1">
+        <v>12345</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2">
+        <v>43790</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>66666</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
+        <v>12398</v>
+      </c>
+      <c r="B7" s="1">
+        <v>32146</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2">
+        <v>43794</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>12399</v>
+      </c>
+      <c r="B8" s="1">
+        <v>12345</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="2">
+        <v>43794</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>12333</v>
+      </c>
+      <c r="B9" s="1">
+        <v>32145</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="2">
+        <v>43794</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>12121</v>
+      </c>
+      <c r="B10" s="1">
+        <v>96325</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="2">
+        <v>43795</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data in excel files
</commit_message>
<xml_diff>
--- a/excel_files/problems.xlsx
+++ b/excel_files/problems.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jscy\Desktop\bootcamp\Schedule-System\excel_files\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
@@ -20,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="15">
   <si>
     <t>problem_id</t>
   </si>
@@ -37,49 +32,40 @@
     <t>description</t>
   </si>
   <si>
-    <t>123456789</t>
-  </si>
-  <si>
-    <t>There are no lights or indications of power</t>
-  </si>
-  <si>
-    <t>Junction box that is uncovered</t>
+    <t>3434T</t>
+  </si>
+  <si>
+    <t>Not working</t>
+  </si>
+  <si>
+    <t>3625N</t>
+  </si>
+  <si>
+    <t>2333B</t>
+  </si>
+  <si>
+    <t>3231R</t>
+  </si>
+  <si>
+    <t>1236G</t>
+  </si>
+  <si>
+    <t>1425F</t>
+  </si>
+  <si>
+    <t>1596D</t>
   </si>
   <si>
     <t>1234A</t>
   </si>
   <si>
-    <t>2333B</t>
-  </si>
-  <si>
-    <t>3231R</t>
-  </si>
-  <si>
-    <t>3434T</t>
-  </si>
-  <si>
-    <t>3625N</t>
-  </si>
-  <si>
-    <t>1236G</t>
-  </si>
-  <si>
-    <t>1425F</t>
-  </si>
-  <si>
-    <t>1596D</t>
-  </si>
-  <si>
     <t>6669R</t>
-  </si>
-  <si>
-    <t>Not working</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -124,9 +110,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -175,7 +158,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -210,7 +193,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -387,7 +370,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -395,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="A1:E1"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,10 +413,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>12346</v>
-      </c>
-      <c r="B2" t="s">
+        <v>12347</v>
+      </c>
+      <c r="B2" s="1">
+        <v>32145</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
+      </c>
+      <c r="D2" s="2">
+        <v>43789</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
@@ -441,21 +430,33 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>12346</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
+        <v>12365</v>
+      </c>
+      <c r="B3" s="1">
+        <v>12345</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2">
+        <v>43790</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>12346</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
+      <c r="B4" s="1">
+        <v>96325</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2">
+        <v>43793</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
@@ -463,21 +464,33 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>12346</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
+        <v>12348</v>
+      </c>
+      <c r="B5" s="1">
+        <v>12347</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2">
+        <v>43794</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>12346</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
+        <v>12398</v>
+      </c>
+      <c r="B6" s="1">
+        <v>32146</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2">
+        <v>43794</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
@@ -485,10 +498,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>12346</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
+        <v>12399</v>
+      </c>
+      <c r="B7" s="1">
+        <v>12345</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="2">
+        <v>43794</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
@@ -496,10 +515,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>12346</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
+        <v>12333</v>
+      </c>
+      <c r="B8" s="1">
+        <v>32145</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2">
+        <v>43794</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
@@ -507,10 +532,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>12346</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
+        <v>12345</v>
+      </c>
+      <c r="B9" s="1">
+        <v>12345</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="2">
+        <v>43795</v>
       </c>
       <c r="E9" t="s">
         <v>6</v>
@@ -518,51 +549,18 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>12346</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
+        <v>12121</v>
+      </c>
+      <c r="B10" s="1">
+        <v>96325</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="2">
+        <v>43795</v>
       </c>
       <c r="E10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>12346</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>12346</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12">
-        <v>1010101010</v>
-      </c>
-      <c r="E12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12346</v>
-      </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13">
-        <v>1010101010</v>
-      </c>
-      <c r="E13" t="s">
         <v>6</v>
       </c>
     </row>
@@ -576,7 +574,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A7" activeCellId="4" sqref="A3:XFD3 A4:XFD4 A5:XFD5 A6:XFD6 A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,138 +605,138 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>12345</v>
+        <v>12347</v>
       </c>
       <c r="B2" s="1">
-        <v>12345</v>
+        <v>32145</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2">
-        <v>43795</v>
+        <v>43789</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>12346</v>
+        <v>12365</v>
       </c>
       <c r="B3" s="1">
-        <v>96325</v>
+        <v>12345</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2">
-        <v>43793</v>
+        <v>43790</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>12348</v>
+        <v>12346</v>
       </c>
       <c r="B4" s="1">
-        <v>12347</v>
+        <v>96325</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2">
-        <v>43794</v>
+        <v>43793</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>12348</v>
+      </c>
+      <c r="B5" s="1">
         <v>12347</v>
       </c>
-      <c r="B5" s="1">
-        <v>32145</v>
-      </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D5" s="2">
-        <v>43789</v>
+        <v>43794</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>12365</v>
+        <v>12398</v>
       </c>
       <c r="B6" s="1">
-        <v>12345</v>
+        <v>32146</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D6" s="2">
-        <v>43790</v>
+        <v>43794</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>12398</v>
+        <v>12399</v>
       </c>
       <c r="B7" s="1">
-        <v>32146</v>
+        <v>12345</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D7" s="2">
         <v>43794</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>12399</v>
+        <v>12333</v>
       </c>
       <c r="B8" s="1">
-        <v>12345</v>
+        <v>32145</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D8" s="2">
         <v>43794</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>12333</v>
+        <v>12345</v>
       </c>
       <c r="B9" s="1">
-        <v>32145</v>
+        <v>12345</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D9" s="2">
-        <v>43794</v>
+        <v>43795</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -749,13 +747,13 @@
         <v>96325</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D10" s="2">
         <v>43795</v>
       </c>
       <c r="E10" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating data in excel files
</commit_message>
<xml_diff>
--- a/excel_files/problems.xlsx
+++ b/excel_files/problems.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="15">
   <si>
     <t>problem_id</t>
   </si>
@@ -32,40 +32,43 @@
     <t>description</t>
   </si>
   <si>
+    <t>2333B</t>
+  </si>
+  <si>
+    <t>Not working</t>
+  </si>
+  <si>
+    <t>3231R</t>
+  </si>
+  <si>
+    <t>1236G</t>
+  </si>
+  <si>
+    <t>1425F</t>
+  </si>
+  <si>
+    <t>1596D</t>
+  </si>
+  <si>
+    <t>1234A</t>
+  </si>
+  <si>
+    <t>6669R</t>
+  </si>
+  <si>
     <t>3434T</t>
   </si>
   <si>
-    <t>Not working</t>
-  </si>
-  <si>
     <t>3625N</t>
-  </si>
-  <si>
-    <t>2333B</t>
-  </si>
-  <si>
-    <t>3231R</t>
-  </si>
-  <si>
-    <t>1236G</t>
-  </si>
-  <si>
-    <t>1425F</t>
-  </si>
-  <si>
-    <t>1596D</t>
-  </si>
-  <si>
-    <t>1234A</t>
-  </si>
-  <si>
-    <t>6669R</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -95,12 +98,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -378,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,16 +417,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>12347</v>
+        <v>12346</v>
       </c>
       <c r="B2" s="1">
-        <v>32145</v>
+        <v>96325</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="2">
-        <v>43789</v>
+        <v>43793</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
@@ -430,16 +434,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>12365</v>
+        <v>12348</v>
       </c>
       <c r="B3" s="1">
-        <v>12345</v>
+        <v>12347</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="2">
-        <v>43790</v>
+        <v>43794</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
@@ -447,16 +451,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>12346</v>
+        <v>12398</v>
       </c>
       <c r="B4" s="1">
-        <v>96325</v>
+        <v>32146</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="2">
-        <v>43793</v>
+        <v>43794</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
@@ -464,10 +468,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>12348</v>
+        <v>12399</v>
       </c>
       <c r="B5" s="1">
-        <v>12347</v>
+        <v>12345</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -481,10 +485,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>12398</v>
+        <v>12333</v>
       </c>
       <c r="B6" s="1">
-        <v>32146</v>
+        <v>32145</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -498,7 +502,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>12399</v>
+        <v>12345</v>
       </c>
       <c r="B7" s="1">
         <v>12345</v>
@@ -507,7 +511,7 @@
         <v>11</v>
       </c>
       <c r="D7" s="2">
-        <v>43794</v>
+        <v>43795</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
@@ -515,16 +519,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>12333</v>
+        <v>12121</v>
       </c>
       <c r="B8" s="1">
-        <v>32145</v>
+        <v>96325</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="2">
-        <v>43794</v>
+        <v>43795</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
@@ -532,35 +536,18 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>12345</v>
+        <v>12121</v>
       </c>
       <c r="B9" s="1">
-        <v>12345</v>
+        <v>96325</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="2">
         <v>43795</v>
       </c>
       <c r="E9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>12121</v>
-      </c>
-      <c r="B10" s="1">
-        <v>96325</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="2">
-        <v>43795</v>
-      </c>
-      <c r="E10" t="s">
         <v>6</v>
       </c>
     </row>
@@ -571,10 +558,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" activeCellId="4" sqref="A3:XFD3 A4:XFD4 A5:XFD5 A6:XFD6 A7:XFD7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,7 +598,7 @@
         <v>32145</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D2" s="2">
         <v>43789</v>
@@ -628,7 +615,7 @@
         <v>12345</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2">
         <v>43790</v>
@@ -639,16 +626,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>12346</v>
-      </c>
-      <c r="B4" s="1">
+        <v>99999</v>
+      </c>
+      <c r="B4">
         <v>96325</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="2">
-        <v>43793</v>
+        <v>12</v>
+      </c>
+      <c r="D4" s="3">
+        <v>43791</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
@@ -656,16 +643,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>12348</v>
-      </c>
-      <c r="B5" s="1">
-        <v>12347</v>
+        <v>99999</v>
+      </c>
+      <c r="B5">
+        <v>96325</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2">
-        <v>43794</v>
+        <v>12</v>
+      </c>
+      <c r="D5" s="3">
+        <v>43791</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
@@ -673,16 +660,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>12398</v>
+        <v>12346</v>
       </c>
       <c r="B6" s="1">
-        <v>32146</v>
+        <v>96325</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D6" s="2">
-        <v>43794</v>
+        <v>43793</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
@@ -690,13 +677,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>12399</v>
+        <v>12348</v>
       </c>
       <c r="B7" s="1">
-        <v>12345</v>
+        <v>12347</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D7" s="2">
         <v>43794</v>
@@ -707,13 +694,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>12333</v>
+        <v>12398</v>
       </c>
       <c r="B8" s="1">
-        <v>32145</v>
+        <v>32146</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D8" s="2">
         <v>43794</v>
@@ -724,16 +711,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>12345</v>
+        <v>12399</v>
       </c>
       <c r="B9" s="1">
         <v>12345</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D9" s="2">
-        <v>43795</v>
+        <v>43794</v>
       </c>
       <c r="E9" t="s">
         <v>6</v>
@@ -741,18 +728,52 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
+        <v>12333</v>
+      </c>
+      <c r="B10" s="1">
+        <v>32145</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="2">
+        <v>43794</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>12345</v>
+      </c>
+      <c r="B11" s="1">
+        <v>12345</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="2">
+        <v>43795</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>12121</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B12" s="1">
         <v>96325</v>
       </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="2">
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="2">
         <v>43795</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E12" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>